<commit_message>
new dataset addded and counting accuracy has been added
</commit_message>
<xml_diff>
--- a/contohpattern.xlsx
+++ b/contohpattern.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamal\Desktop\TA NOPAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project(s)\Perjokian duniawi\TA NOPAL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BF20B8-6606-4F70-BED4-B5BDDA160492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B68ED7-CE20-4530-871F-A7AB55D2A73E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-2400" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>namapattern</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>please open</t>
+  </si>
+  <si>
+    <t>Dear Sir</t>
   </si>
 </sst>
 </file>
@@ -405,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,6 +509,11 @@
         <v>14</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>